<commit_message>
Moved routes into its own file and added some tools that will be useful when using passport.js.
</commit_message>
<xml_diff>
--- a/notes/apis.xlsx
+++ b/notes/apis.xlsx
@@ -87,9 +87,6 @@
     <t>/register/</t>
   </si>
   <si>
-    <t>restrictBy: userId, date; sortBy: date, alphanumeric</t>
-  </si>
-  <si>
     <t>sortBy: date, alphanumeric, restrictBy: campaignId, date</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>/campaigns/:campaign_id</t>
+  </si>
+  <si>
+    <t>restrictBy: userId, date; sortBy: date, alphanumeric; include: all, campaignId</t>
   </si>
 </sst>
 </file>
@@ -499,7 +499,7 @@
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -534,12 +534,12 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>8</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="7" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
@@ -592,7 +592,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -641,7 +641,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
@@ -661,12 +661,12 @@
         <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>3</v>
@@ -677,7 +677,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -688,7 +688,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
@@ -719,34 +719,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>